<commit_message>
Well, none of this works anymore.
</commit_message>
<xml_diff>
--- a/Programming for Finance/Lecture 4/data.xlsx
+++ b/Programming for Finance/Lecture 4/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpfif\Documents\Python\Programming for Finance\Lecture 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpfif\Documents\Python\misc-python\Programming for Finance\Lecture 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -838,7 +838,7 @@
   <dimension ref="A1:C6246"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -862,7 +862,7 @@
         <v>100</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -873,7 +873,7 @@
         <v>401</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -881,7 +881,7 @@
         <v>42770</v>
       </c>
       <c r="B4">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -903,7 +903,7 @@
         <v>42768</v>
       </c>
       <c r="B6">
-        <v>610</v>
+        <v>408</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -914,7 +914,7 @@
         <v>42767</v>
       </c>
       <c r="B7">
-        <v>200</v>
+        <v>800</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -925,7 +925,7 @@
         <v>42766</v>
       </c>
       <c r="B8">
-        <v>245</v>
+        <v>200</v>
       </c>
       <c r="C8">
         <v>0</v>

</xml_diff>